<commit_message>
Add new publisher column to template
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dwijnbergen\OneDrive - LUMC\PhD\private\table-to-rdf\file_structure\FDP_WP13\catalog_IBM_omics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://lumconline-my.sharepoint.com/personal/j_d_wijnbergen_lumc_nl/Documents/PhD/private/table-to-rdf/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2321211D-1962-41CC-AA5A-D80A53A84211}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="105" documentId="13_ncr:1_{F121C1B1-7B55-4B5D-A7F0-2C0417290B66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7711D102-29FD-47E8-B4A0-3CBA349F2FE9}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="datasets.csv" sheetId="2" r:id="rId1"/>
     <sheet name="distributions.csv" sheetId="1" r:id="rId2"/>
-    <sheet name="Languages" sheetId="3" r:id="rId3"/>
-    <sheet name="Mediatypes" sheetId="5" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId3"/>
+    <sheet name="Languages" sheetId="3" r:id="rId4"/>
+    <sheet name="Mediatypes" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6476" uniqueCount="5482">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6481" uniqueCount="5486">
   <si>
     <t>application/gzip</t>
   </si>
@@ -16479,6 +16480,18 @@
   </si>
   <si>
     <t>CompressionFormat</t>
+  </si>
+  <si>
+    <t>https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE151757</t>
+  </si>
+  <si>
+    <t>https://ftp.ncbi.nlm.nih.gov/geo/series/GSE151nnn/GSE151757/suppl/GSE151757_raw_counts.txt.gz</t>
+  </si>
+  <si>
+    <t>https://ftp.ncbi.nlm.nih.gov/geo/series/GSE151nnn/GSE151757/suppl/GSE151757_DESeq2_normalized_counts.txt.gz</t>
+  </si>
+  <si>
+    <t>https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE151758</t>
   </si>
 </sst>
 </file>
@@ -16635,7 +16648,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -16821,8 +16834,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor theme="6" tint="0.59999389629810485"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor theme="6" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -16937,6 +16962,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -16983,7 +17023,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
@@ -17002,13 +17042,14 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" quotePrefix="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -17055,7 +17096,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="25">
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
       <fill>
@@ -17126,6 +17167,14 @@
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
         </patternFill>
       </fill>
     </dxf>
@@ -17285,32 +17334,33 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B1316F4C-BBAB-465C-97A2-E82F20FD80AC}" name="Table2" displayName="Table2" ref="A1:I20" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B1316F4C-BBAB-465C-97A2-E82F20FD80AC}" name="Table2" displayName="Table2" ref="A1:I20" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
   <autoFilter ref="A1:I20" xr:uid="{289BF9AA-09AB-49BF-8A8C-03CEF2C0C744}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I4">
     <sortCondition ref="A1:A20"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{B12F2A67-A802-4A1D-A507-CD1A81259F21}" name="Title*" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{DB6FE244-75C4-4106-A109-2175F9085F14}" name="Publisher*" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{017BBF02-2796-448B-AEE4-0E2F98781F35}" name="Description" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{A2B9F66D-A060-47A8-96EE-B8378B8306FE}" name="Language" dataDxfId="18"/>
-    <tableColumn id="5" xr3:uid="{ECADE6F1-E3F2-4862-B6DD-ABA490BF9DBC}" name="License" dataDxfId="17"/>
-    <tableColumn id="9" xr3:uid="{0DC64F86-319D-47A3-8B35-0E0FF21892AB}" name="ContactPoint" dataDxfId="16"/>
-    <tableColumn id="10" xr3:uid="{F3845B1C-7167-4EFF-80BA-0B2FCF86369C}" name="LandingPage" dataDxfId="15"/>
-    <tableColumn id="11" xr3:uid="{015B6BB7-DFA0-4CB7-9C85-057381C2995E}" name="Keywords" dataDxfId="14"/>
-    <tableColumn id="12" xr3:uid="{E14A609D-1A0D-4142-BC8C-EBA69952A394}" name="Themes*" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{B12F2A67-A802-4A1D-A507-CD1A81259F21}" name="Title*" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{DB6FE244-75C4-4106-A109-2175F9085F14}" name="Publisher*" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{017BBF02-2796-448B-AEE4-0E2F98781F35}" name="Description" dataDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{A2B9F66D-A060-47A8-96EE-B8378B8306FE}" name="Language" dataDxfId="19"/>
+    <tableColumn id="5" xr3:uid="{ECADE6F1-E3F2-4862-B6DD-ABA490BF9DBC}" name="License" dataDxfId="18"/>
+    <tableColumn id="9" xr3:uid="{0DC64F86-319D-47A3-8B35-0E0FF21892AB}" name="ContactPoint" dataDxfId="17"/>
+    <tableColumn id="10" xr3:uid="{F3845B1C-7167-4EFF-80BA-0B2FCF86369C}" name="LandingPage" dataDxfId="16"/>
+    <tableColumn id="11" xr3:uid="{015B6BB7-DFA0-4CB7-9C85-057381C2995E}" name="Keywords" dataDxfId="15"/>
+    <tableColumn id="12" xr3:uid="{E14A609D-1A0D-4142-BC8C-EBA69952A394}" name="Themes*" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F568F700-D70A-44C8-B20C-EA224B57BBE9}" name="Table3" displayName="Table3" ref="A1:K20" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
-  <autoFilter ref="A1:K20" xr:uid="{43EEDAAA-0476-4939-82F6-F6D169F223C3}"/>
-  <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{7ED86CA5-C622-428D-A7D4-43B6C9AB850A}" name="Title*" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{DB4F9D13-7765-46FE-94CC-860ABAE684E2}" name="Dataset title*" dataDxfId="9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F568F700-D70A-44C8-B20C-EA224B57BBE9}" name="Table3" displayName="Table3" ref="A1:L20" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+  <autoFilter ref="A1:L20" xr:uid="{43EEDAAA-0476-4939-82F6-F6D169F223C3}"/>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{7ED86CA5-C622-428D-A7D4-43B6C9AB850A}" name="Title*" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{DB4F9D13-7765-46FE-94CC-860ABAE684E2}" name="Dataset title*" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{3D86FDF1-081A-4A4F-AC06-DAD32F3F8AC0}" name="Publisher*" dataDxfId="9" dataCellStyle="Hyperlink"/>
     <tableColumn id="4" xr3:uid="{27E9BBD6-A1D4-4278-B4D7-87497FA7B8B7}" name="Description" dataDxfId="8"/>
     <tableColumn id="5" xr3:uid="{31797BFE-51FD-406F-9580-AF4D21A97FBB}" name="Language" dataDxfId="7"/>
     <tableColumn id="6" xr3:uid="{D42920E6-BEC9-49FD-873F-94DF99D4BC34}" name="License" dataDxfId="6"/>
@@ -17624,22 +17674,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{441B2AFF-9841-4F9B-AF59-44C0E5F67318}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I30" sqref="I30"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="63.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.28515625" style="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25.7109375" style="8" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="55.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="76.140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="133" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="255.7109375" style="17" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="32.140625" style="8" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="76.140625" style="8" bestFit="1" customWidth="1"/>
     <col min="12" max="16384" width="8.85546875" style="8"/>
@@ -17676,53 +17726,53 @@
     </row>
     <row r="2" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
-      <c r="B2" s="14"/>
+      <c r="B2" s="7"/>
       <c r="C2" s="13"/>
       <c r="D2" s="13"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
       <c r="H2" s="13"/>
       <c r="I2" s="13"/>
     </row>
     <row r="3" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
-      <c r="B3" s="14"/>
+      <c r="B3" s="7"/>
       <c r="C3" s="13"/>
       <c r="D3" s="13"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
       <c r="H3" s="13"/>
       <c r="I3" s="13"/>
     </row>
     <row r="4" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
-      <c r="B4" s="14"/>
+      <c r="B4" s="7"/>
       <c r="C4" s="13"/>
       <c r="D4" s="13"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
       <c r="H4" s="13"/>
       <c r="I4" s="13"/>
     </row>
     <row r="5" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13"/>
-      <c r="B5" s="14"/>
+      <c r="B5" s="7"/>
       <c r="C5" s="13"/>
       <c r="D5" s="13"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="16"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="15"/>
       <c r="H5" s="13"/>
-      <c r="I5" s="16"/>
+      <c r="I5" s="13"/>
     </row>
     <row r="6" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
-      <c r="B6" s="6"/>
+      <c r="B6" s="7"/>
       <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
+      <c r="D6" s="13"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
@@ -17731,9 +17781,9 @@
     </row>
     <row r="7" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
-      <c r="B7" s="6"/>
+      <c r="B7" s="7"/>
       <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
+      <c r="D7" s="13"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
@@ -17930,18 +17980,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K41"/>
+  <dimension ref="A1:L41"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="16.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.7109375" style="10" customWidth="1"/>
+    <col min="2" max="2" width="34.42578125" style="10" customWidth="1"/>
     <col min="3" max="3" width="63.85546875" style="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" style="10" customWidth="1"/>
     <col min="6" max="6" width="54.5703125" style="10" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="118.5703125" style="10" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17" style="10" bestFit="1" customWidth="1"/>
@@ -17953,287 +18004,309 @@
     <col min="14" max="16384" width="8.85546875" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>5481</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="13"/>
       <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
+      <c r="C2" s="7"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
-      <c r="F2" s="5"/>
+      <c r="F2" s="4"/>
       <c r="G2" s="5"/>
-      <c r="H2"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="12"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
+      <c r="H2" s="5"/>
+      <c r="I2"/>
+      <c r="J2"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="12"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="13"/>
       <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
+      <c r="C3" s="7"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
       <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="12"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
+      <c r="J3"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="12"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="13"/>
       <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
+      <c r="C4" s="7"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
+      <c r="G4" s="5"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
-      <c r="K4" s="12"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="12"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="13"/>
       <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
+      <c r="C5" s="7"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
+      <c r="G5" s="5"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
-      <c r="K5" s="12"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="12"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="13"/>
       <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
+      <c r="C6" s="7"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
+      <c r="G6" s="5"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
-      <c r="K6" s="12"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="12"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="13"/>
       <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
+      <c r="C7" s="7"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
+      <c r="G7" s="5"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
-      <c r="K7" s="12"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="12"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="13"/>
       <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
+      <c r="C8" s="7"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
+      <c r="G8" s="5"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
-      <c r="K8" s="12"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="12"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="13"/>
       <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
+      <c r="C9" s="7"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
+      <c r="G9" s="5"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
-      <c r="K9" s="12"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="12"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="13"/>
       <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
+      <c r="C10" s="7"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
+      <c r="G10" s="5"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
-      <c r="K10" s="12"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="12"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="13"/>
       <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
+      <c r="C11" s="7"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
+      <c r="G11" s="5"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
-      <c r="K11" s="12"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="12"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="13"/>
       <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
+      <c r="C12" s="7"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
+      <c r="G12" s="5"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
-      <c r="K12" s="12"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="12"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="13"/>
       <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
+      <c r="C13" s="7"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
+      <c r="G13" s="5"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
-      <c r="K13" s="12"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="12"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="13"/>
       <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
+      <c r="C14" s="7"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
+      <c r="G14" s="5"/>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
-      <c r="K14" s="12"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="12"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="13"/>
       <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
+      <c r="C15" s="7"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
+      <c r="G15" s="5"/>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
-      <c r="K15" s="12"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="12"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="13"/>
       <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
+      <c r="C16" s="7"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
+      <c r="G16" s="5"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
-      <c r="K16" s="12"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="12"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="13"/>
       <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
+      <c r="C17" s="7"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
+      <c r="G17" s="5"/>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
-      <c r="K17" s="12"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="12"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="13"/>
       <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
+      <c r="C18" s="7"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="5"/>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
-      <c r="K18" s="12"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="12"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="13"/>
       <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
+      <c r="C19" s="7"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
       <c r="G19" s="5"/>
-      <c r="H19" s="4"/>
+      <c r="H19" s="5"/>
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
-      <c r="K19" s="12"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="12"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="13"/>
       <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
+      <c r="C20" s="7"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
-      <c r="F20" s="5"/>
+      <c r="F20" s="4"/>
       <c r="G20" s="5"/>
-      <c r="H20" s="4"/>
+      <c r="H20" s="5"/>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
-      <c r="K20" s="12"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="12"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="8"/>
@@ -18247,24 +18320,28 @@
       <c r="K41" s="8"/>
     </row>
   </sheetData>
+  <sheetProtection insertRows="0" selectLockedCells="1"/>
   <phoneticPr fontId="19" type="noConversion"/>
-  <dataValidations xWindow="168" yWindow="713" count="7">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Description" prompt="Description of the distribution with the language tag" sqref="C2:C20" xr:uid="{07D38365-DD9A-4859-A53E-4F891F44F67D}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Format" prompt="Format" sqref="J2:J20" xr:uid="{519B8B6D-8231-46DC-BEBD-316308A32CF4}"/>
-    <dataValidation type="custom" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must start with &quot;http://&quot; or &quot;https://&quot;" promptTitle="License" prompt="License of the resource. For example, https://creativecommons.org/licenses/by/4.0/deed.en_x000a__x000a_Must start with &quot;http://&quot; or &quot;https://&quot;" sqref="E2:E20" xr:uid="{BB47F515-A56C-4F49-8BE1-04D7789A3F47}">
-      <formula1>OR(LEFT(E2,7)="http://", LEFT(E2,8)="https://")</formula1>
+  <dataValidations xWindow="131" yWindow="305" count="8">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Description" prompt="Description of the distribution with the language tag" sqref="D2:D20" xr:uid="{D0717FC4-7DC1-40F6-B33B-C5D4C4D33EA4}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Format" prompt="Format" sqref="K2:K20" xr:uid="{6C320EA0-FA35-4E5C-8497-B67F948F8686}"/>
+    <dataValidation type="custom" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must start with &quot;http://&quot; or &quot;https://&quot;" promptTitle="License" prompt="License of the resource. For example, https://creativecommons.org/licenses/by/4.0/deed.en_x000a__x000a_Must start with &quot;http://&quot; or &quot;https://&quot;" sqref="F2:F20" xr:uid="{019BF7F4-D7F1-4E53-B0DA-4F6B2D2A2DD4}">
+      <formula1>OR(LEFT(F2,7)="http://", LEFT(F2,8)="https://")</formula1>
     </dataValidation>
-    <dataValidation type="custom" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be a positive integer" promptTitle="Bytesize" prompt="The size of the distribution in bytes_x000a__x000a_Must be a positive integer" sqref="K2:K20" xr:uid="{6ABA25F5-30EA-447E-B7ED-5C1C16CE953E}">
-      <formula1>AND(ISNUMBER(K2), INT(K2) = K2, K2 &gt;= 0)</formula1>
+    <dataValidation type="custom" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be a positive integer" promptTitle="Bytesize" prompt="The size of the distribution in bytes_x000a__x000a_Must be a positive integer" sqref="L2:L20" xr:uid="{ED29D748-8023-43A2-AE72-5BE2518C8CF0}">
+      <formula1>AND(ISNUMBER(L2), INT(L2) = L2, L2 &gt;= 0)</formula1>
     </dataValidation>
-    <dataValidation type="custom" errorStyle="warning" showInputMessage="1" showErrorMessage="1" error="Required field" promptTitle="Title" prompt="Name of the data distribution with the language tag_x000a__x000a_Required field" sqref="A2:A20" xr:uid="{08BFD649-99E0-43F9-B81D-3458ED59BCA0}">
-      <formula1>LEN(A2) &gt;= IF((SUM(LEN(B2:J2)) &gt;= 1),1,0)</formula1>
+    <dataValidation type="custom" errorStyle="warning" showInputMessage="1" showErrorMessage="1" error="One of AccessURL or DownloadURL is required. Must start with &quot;http://&quot;, &quot;https://&quot; or &quot;ftp://&quot;" promptTitle="AccessURL" prompt="A landing page, feed, SPARQL endpoint or other type of resource that gives access to the distribution of the dataset_x000a__x000a_One of AccessURL or DownloadURL is required. Must start with &quot;http://&quot;, &quot;https://&quot; or &quot;ftp://&quot;" sqref="G2:G20" xr:uid="{5BDE2F96-7DBE-49C1-96B8-7E7B52FEC7A6}">
+      <formula1>OR(AND(LEN(G2) &gt;= IF((SUM(LEN(A2:L2)) &gt;= 1),1,0), OR(LEFT(G2,7)="http://", LEFT(G2,8)="https://", LEFT(G2,6) =  "ftp://", SUM(LEN(A2:L2)) = 0)), OR(LEFT(H2,7)="http://", LEFT(H2,8)="https://", LEFT(H2,6) =  "ftp://"))</formula1>
     </dataValidation>
-    <dataValidation type="custom" errorStyle="warning" showInputMessage="1" showErrorMessage="1" error="One of AccessURL or DownloadURL is required. Must start with &quot;http://&quot;, &quot;https://&quot; or &quot;ftp://&quot;" promptTitle="AccessURL" prompt="A landing page, feed, SPARQL endpoint or other type of resource that gives access to the distribution of the dataset_x000a__x000a_One of AccessURL or DownloadURL is required. Must start with &quot;http://&quot;, &quot;https://&quot; or &quot;ftp://&quot;" sqref="F2:F20" xr:uid="{8947F337-11F6-411C-B02E-4FDED69BBE8B}">
-      <formula1>OR(AND(LEN(F2) &gt;= IF((SUM(LEN(A2:K2)) &gt;= 1),1,0), OR(LEFT(F2,7)="http://", LEFT(F2,8)="https://", LEFT(F2,6) =  "ftp://", SUM(LEN(A2:K2)) = 0)), OR(LEFT(G2,7)="http://", LEFT(G2,8)="https://", LEFT(G2,6) =  "ftp://"))</formula1>
+    <dataValidation type="custom" errorStyle="warning" showInputMessage="1" showErrorMessage="1" error="One of AccessURL or DownloadURL is required. Must start with &quot;http://&quot;, &quot;https://&quot; or &quot;ftp://&quot;" promptTitle="DownloadURL" prompt="A file that contains the distribution of the dataset in a given format_x000a__x000a_One of AccessURL or DownloadURL is required. Must start with &quot;http://&quot;, &quot;https://&quot; or &quot;ftp://&quot;" sqref="H2:H20" xr:uid="{AA4DDEF3-73EC-45CC-85F1-E2F32BEE81B1}">
+      <formula1>OR(AND(LEN(H2) &gt;= IF((SUM(LEN(A2:L2)) &gt;= 1),1,0), OR(LEFT(H2,7)="http://", LEFT(H2,8)="https://", LEFT(H2,6) =  "ftp://", SUM(LEN(A2:L2)) = 0)),  OR(LEFT(G2,7)="http://", LEFT(G2,8)="https://", LEFT(G2,6) =  "ftp://"))</formula1>
     </dataValidation>
-    <dataValidation type="custom" errorStyle="warning" showInputMessage="1" showErrorMessage="1" error="One of AccessURL or DownloadURL is required. Must start with &quot;http://&quot;, &quot;https://&quot; or &quot;ftp://&quot;" promptTitle="DownloadURL" prompt="A file that contains the distribution of the dataset in a given format_x000a__x000a_One of AccessURL or DownloadURL is required. Must start with &quot;http://&quot;, &quot;https://&quot; or &quot;ftp://&quot;" sqref="G2:G20" xr:uid="{E897DE77-542B-444C-A050-BECEE15CDF3D}">
-      <formula1>OR(AND(LEN(G2) &gt;= IF((SUM(LEN(A2:K2)) &gt;= 1),1,0), OR(LEFT(G2,7)="http://", LEFT(G2,8)="https://", LEFT(G2,6) =  "ftp://", SUM(LEN(A2:K2)) = 0)),  OR(LEFT(F2,7)="http://", LEFT(F2,8)="https://", LEFT(F2,6) =  "ftp://"))</formula1>
+    <dataValidation type="custom" errorStyle="warning" showInputMessage="1" showErrorMessage="1" error="Required field, must start with &quot;https://orcid.org/&quot;" promptTitle="Publisher" prompt="ORCID ID of Organisation(s) or Persons(s) responsible for the dataset._x000a_Required field, must start with &quot;https://orcid.org/&quot;" sqref="C2:C20" xr:uid="{65B94768-83C6-436B-A0C5-D9BEE4D50DA9}">
+      <formula1>AND(LEN(C2) &gt;= IF((SUM(LEN(A2:L2)) &gt;= 1),1,0), OR(LEFT(C2,18)="https://orcid.org/", SUM(LEN(B2:J2)) = 0))</formula1>
+    </dataValidation>
+    <dataValidation type="custom" errorStyle="warning" showInputMessage="1" showErrorMessage="1" error="Mandatory field" promptTitle="Title" prompt="Name of the dataset with the language tag_x000a__x000a_Mandatory field" sqref="A2:A20" xr:uid="{2ADD73F9-72DC-434D-AB03-77CD135FE7DD}">
+      <formula1>LEN(A2) &gt;= IF((SUM(LEN(A2:L2)) &gt;= 1),1,0)</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18274,30 +18351,30 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="168" yWindow="713" count="4">
-        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Required field. Must be the title of a dataset in the datasets sheet" promptTitle="Dataset title" prompt="Title of the dataset associated with the distribution_x000a__x000a_Required field. Must be the title of a dataset in the datasets sheet" xr:uid="{7FE47C44-51FE-401E-B5E2-E4DC5F18FCC0}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="131" yWindow="305" count="4">
+        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="_x000a_Must be media type from https://www.iana.org/assignments/media-types/media-types.xhtml" promptTitle="MediaType" prompt="The media type of the distribution_x000a__x000a_Must be media type from https://www.iana.org/assignments/media-types/media-types.xhtml" xr:uid="{2D29C53A-7574-4616-A6E8-2D9A42ED8503}">
           <x14:formula1>
-            <xm:f>datasets.csv!$A$2:$A$20</xm:f>
+            <xm:f>Mediatypes!$B$2:$B$1910</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B20</xm:sqref>
+          <xm:sqref>J2:J20</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="_x000a_Must be media type from https://www.iana.org/assignments/media-types/media-types.xhtml" promptTitle="MediaType" prompt="The media type of the distribution_x000a__x000a_Must be media type from https://www.iana.org/assignments/media-types/media-types.xhtml" xr:uid="{0436649A-F0A9-4C05-8BB8-12535E0E8D37}">
+        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be two letter language code from https://id.loc.gov/vocabulary/iso639-1.html" promptTitle="Language" prompt="Language of the dataset_x000a__x000a__x000a_Must be two letter language code from https://id.loc.gov/vocabulary/iso639-1.html" xr:uid="{9C3A6ADC-696A-43C1-9842-B983BA15890C}">
+          <x14:formula1>
+            <xm:f>Languages!$B$2:$B$185</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:E20</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Required field. Must be media type from https://www.iana.org/assignments/media-types/media-types.xhtml" promptTitle="MediaType" prompt="The media type of the distribution_x000a__x000a_Required field. Must be media type from https://www.iana.org/assignments/media-types/media-types.xhtml" xr:uid="{B522617B-407F-4ACE-A865-D3490D785DBE}">
           <x14:formula1>
             <xm:f>Mediatypes!$B$2:$B$1910</xm:f>
           </x14:formula1>
           <xm:sqref>I2:I20</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be two letter language code from https://id.loc.gov/vocabulary/iso639-1.html" promptTitle="Language" prompt="Language of the dataset_x000a__x000a__x000a_Must be two letter language code from https://id.loc.gov/vocabulary/iso639-1.html" xr:uid="{4801E933-C089-4043-9B74-29ECF730C594}">
+        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Required field. Must be the title of a dataset in the datasets sheet" promptTitle="Dataset title" prompt="Title of the dataset associated with the distribution_x000a__x000a_Required field. Must be the title of a dataset in the datasets sheet" xr:uid="{AE71F0C5-86B8-4E09-B4FC-F29E70BA6DEE}">
           <x14:formula1>
-            <xm:f>Languages!$B$2:$B$185</xm:f>
+            <xm:f>datasets.csv!$A$2:$A$20</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D20</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Required field. Must be media type from https://www.iana.org/assignments/media-types/media-types.xhtml" promptTitle="MediaType" prompt="The media type of the distribution_x000a__x000a_Required field. Must be media type from https://www.iana.org/assignments/media-types/media-types.xhtml" xr:uid="{5C121557-C047-4315-865E-DF769FF7433F}">
-          <x14:formula1>
-            <xm:f>Mediatypes!$B$2:$B$1910</xm:f>
-          </x14:formula1>
-          <xm:sqref>H2:H20</xm:sqref>
+          <xm:sqref>B5:B20 B2:B3</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -18306,11 +18383,53 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEE51EC6-F875-417F-8395-9D968508445C}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>5482</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>5483</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>5485</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>5484</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="custom" errorStyle="warning" showInputMessage="1" showErrorMessage="1" error="One of AccessURL or DownloadURL is required. Must start with &quot;http://&quot;, &quot;https://&quot; or &quot;ftp://&quot;" promptTitle="DownloadURL" prompt="A file that contains the distribution of the dataset in a given format_x000a__x000a_One of AccessURL or DownloadURL is required. Must start with &quot;http://&quot;, &quot;https://&quot; or &quot;ftp://&quot;" sqref="B1:B2" xr:uid="{955874C5-2040-4C41-8AA7-88F4E8F03615}">
+      <formula1>OR(AND(LEN(B1) &gt;= IF((SUM(LEN(F1:XEY1)) &gt;= 1),1,0), OR(LEFT(B1,7)="http://", LEFT(B1,8)="https://", LEFT(B1,6) =  "ftp://", SUM(LEN(F1:XEY1)) = 0)),  OR(LEFT(A1,7)="http://", LEFT(A1,8)="https://", LEFT(A1,6) =  "ftp://"))</formula1>
+    </dataValidation>
+    <dataValidation type="custom" errorStyle="warning" showInputMessage="1" showErrorMessage="1" error="One of AccessURL or DownloadURL is required. Must start with &quot;http://&quot;, &quot;https://&quot; or &quot;ftp://&quot;" promptTitle="AccessURL" prompt="A landing page, feed, SPARQL endpoint or other type of resource that gives access to the distribution of the dataset_x000a__x000a_One of AccessURL or DownloadURL is required. Must start with &quot;http://&quot;, &quot;https://&quot; or &quot;ftp://&quot;" sqref="A1:A2" xr:uid="{7F7C952E-1231-448C-8569-29742C2E670B}">
+      <formula1>OR(AND(LEN(A1) &gt;= IF((SUM(LEN(F1:XEY1)) &gt;= 1),1,0), OR(LEFT(A1,7)="http://", LEFT(A1,8)="https://", LEFT(A1,6) =  "ftp://", SUM(LEN(F1:XEY1)) = 0)), OR(LEFT(B1,7)="http://", LEFT(B1,8)="https://", LEFT(B1,6) =  "ftp://"))</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{3DB1250C-1350-46EB-883A-2D8DFCB7866B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F332B04E-55DA-4BCC-BF87-5100CD393BE7}">
   <dimension ref="A1:J185"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B117" sqref="B117"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20918,17 +21037,18 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{844781CE-CFAE-4361-A920-ACB28080BD5B}">
   <dimension ref="A1:C1910"/>
   <sheetViews>
-    <sheetView topLeftCell="A226" workbookViewId="0">
-      <selection activeCell="B242" sqref="B242"/>
+    <sheetView topLeftCell="A1749" workbookViewId="0">
+      <selection activeCell="A1762" sqref="A1762"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -41907,6 +42027,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>